<commit_message>
SQL Server Interview Questions and Answers
Studied recursive query statements, join differences, practiced sql.
Wanted to study something different today
</commit_message>
<xml_diff>
--- a/git command organized.xlsx
+++ b/git command organized.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="36" windowWidth="23280" windowHeight="11592" tabRatio="590"/>
+    <workbookView xWindow="360" yWindow="36" windowWidth="23256" windowHeight="11592" tabRatio="590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -387,6 +386,61 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Image result for git branching strategy"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4693920" y="19667220"/>
+          <a:ext cx="5684520" cy="3649980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -647,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -657,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>